<commit_message>
AtlasOfLivingAustralia/biocollect#1759 - fixes bug with empty table throwing an error
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk_import_example.xlsx
+++ b/src/test/resources/bulk_import_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/var03f/git/ecodata/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE5A5FC-0D3D-B14B-B43C-35BD46C479B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04108F48-F127-E94D-96BD-FA2710F3BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24400" yWindow="1120" windowWidth="18960" windowHeight="31600" xr2:uid="{2C3550E1-BCA6-BC4F-80D3-E9595D4DE580}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26560" xr2:uid="{2C3550E1-BCA6-BC4F-80D3-E9595D4DE580}"/>
   </bookViews>
   <sheets>
     <sheet name="form1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>serial</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>gi5</t>
+  </si>
+  <si>
+    <t>test a 3</t>
+  </si>
+  <si>
+    <t>test bc 6</t>
   </si>
 </sst>
 </file>
@@ -288,9 +294,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -328,7 +334,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -434,7 +440,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -576,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2094674-6F1F-0348-B85A-E3F91D4F3835}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,6 +866,27 @@
         <v>58</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AtlasOfLivingAustralia/biocollect#1759 - added another example
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk_import_example.xlsx
+++ b/src/test/resources/bulk_import_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/var03f/git/ecodata/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04108F48-F127-E94D-96BD-FA2710F3BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769E5EA-E90F-E141-96BB-092F5B0496A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26560" xr2:uid="{2C3550E1-BCA6-BC4F-80D3-E9595D4DE580}"/>
   </bookViews>
@@ -590,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2094674-6F1F-0348-B85A-E3F91D4F3835}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,6 +887,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>